<commit_message>
Align WHO Hepatitis B and Hib with current WHO/CDC guidance
- HepB: fix Dose 3 absMinAge 14wk -> 24wk, absMinInt 4wk -> 8wk from
  Dose 2, add 16-week minimum interval constraint from Dose 1 to Dose 3
- Hib: remove discontinued HbOC vaccine (CVX 47), add 4-dose series
  (3p+1 with booster at 12-15mo) as alternative to 3p+0 primary series

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/cicada_generator/lib/WHO/antigen/HepB.xlsx
+++ b/cicada_generator/lib/WHO/antigen/HepB.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="40">
   <si>
     <t xml:space="preserve">Clinical History Immunity</t>
   </si>
@@ -126,10 +126,13 @@
     <t xml:space="preserve">Dose 3</t>
   </si>
   <si>
-    <t xml:space="preserve">14 weeks</t>
+    <t xml:space="preserve">24 weeks</t>
   </si>
   <si>
     <t xml:space="preserve">8 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 weeks</t>
   </si>
 </sst>
 </file>
@@ -506,12 +509,6 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -641,12 +638,6 @@
       <c r="F17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
@@ -676,15 +667,6 @@
       <c r="I18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
@@ -823,12 +805,6 @@
       <c r="F27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
@@ -847,10 +823,10 @@
         <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>38</v>
@@ -858,25 +834,16 @@
       <c r="I28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>10</v>
@@ -885,10 +852,16 @@
         <v>10</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30">
@@ -896,10 +869,10 @@
         <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>10</v>
@@ -911,21 +884,30 @@
         <v>10</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="32">
@@ -933,10 +915,10 @@
         <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>10</v>
@@ -947,7 +929,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>19</v>
@@ -961,10 +943,10 @@
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>10</v>
@@ -972,9 +954,23 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>